<commit_message>
adding changing background feature
</commit_message>
<xml_diff>
--- a/renderer/Template_Database.xlsx
+++ b/renderer/Template_Database.xlsx
@@ -440,6 +440,12 @@
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>SEPEDAH</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -451,12 +457,6 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>Mattel</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -479,6 +479,12 @@
       <c r="C6">
         <v>5</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="str">
+        <v>SEPEDAH</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -501,12 +507,6 @@
       <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>Mattel</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -517,6 +517,12 @@
       </c>
       <c r="C9">
         <v>8</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>BARBIE KEREN</v>
       </c>
     </row>
     <row r="10">

</xml_diff>